<commit_message>
prepare publication 3.1.0 (#114)
* prepare publication and update workflow

* refacto index

* refacto index

* refacto index af261ff599183521f98264e944b24c6244726079
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-mesures-diabetis-type.xlsx
+++ b/main/ig/StructureDefinition-mesures-diabetis-type.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-10-02T08:33:33+00:00</t>
+    <t>2024-10-02T08:34:04+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1121,7 +1121,7 @@
         <v>78</v>
       </c>
       <c r="AI4" t="s" s="2">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="AJ4" t="s" s="2">
         <v>81</v>
@@ -1327,7 +1327,7 @@
         <v>83</v>
       </c>
       <c r="AI6" t="s" s="2">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="AJ6" t="s" s="2">
         <v>108</v>

</xml_diff>